<commit_message>
WeatherAPI.com entegrasyonu - Gerçek hava durumu verileri eklendi
</commit_message>
<xml_diff>
--- a/data/mac-sonuclari.xlsx
+++ b/data/mac-sonuclari.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yakay\OneDrive\Masaüstü\d-8\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{357554EF-3CAA-4A83-AFA3-74BD1524386A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FECE4BD-187B-48FA-A05E-F9CE2224BE17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="22">
   <si>
     <t>Tarih</t>
   </si>
@@ -467,7 +467,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -674,13 +674,73 @@
         <v>10</v>
       </c>
     </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>45833</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.875</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>45833</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="2"/>
+      <c r="A12" s="1">
+        <v>45834</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0.875</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="2"/>
+      <c r="A13" s="1">
+        <v>45834</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
@@ -709,7 +769,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:G1 C2 E2" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:G1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
23.06.2025 - Fortuna United vs Ofside
</commit_message>
<xml_diff>
--- a/data/mac-sonuclari.xlsx
+++ b/data/mac-sonuclari.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yakay\OneDrive\Masaüstü\d-8\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FECE4BD-187B-48FA-A05E-F9CE2224BE17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48CCB0DE-F053-413E-A614-C7E4726B56C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -467,7 +467,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -656,6 +656,12 @@
       <c r="E8" t="s">
         <v>19</v>
       </c>
+      <c r="F8">
+        <v>6</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">

</xml_diff>

<commit_message>
23.06.2025 - maç sonuçları
</commit_message>
<xml_diff>
--- a/data/mac-sonuclari.xlsx
+++ b/data/mac-sonuclari.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yakay\OneDrive\Masaüstü\d-8\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48CCB0DE-F053-413E-A614-C7E4726B56C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D90EC2D1-E1A3-4884-AAD9-AF9A802D0BF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -85,7 +85,7 @@
     <t>61.Alay</t>
   </si>
   <si>
-    <t>Fortuna Unıted</t>
+    <t>Fortuna United</t>
   </si>
 </sst>
 </file>
@@ -467,7 +467,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -679,6 +679,12 @@
       <c r="E9" t="s">
         <v>10</v>
       </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">

</xml_diff>

<commit_message>
oynanacak maçlar eklendi - 3 Temmuz maçları
</commit_message>
<xml_diff>
--- a/data/mac-sonuclari.xlsx
+++ b/data/mac-sonuclari.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yakay\OneDrive\Masaüstü\d-8\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D90EC2D1-E1A3-4884-AAD9-AF9A802D0BF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02EE8AAE-DCB6-4591-8867-6582502EE88E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="22">
   <si>
     <t>Tarih</t>
   </si>
@@ -467,7 +467,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -755,28 +755,106 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="2"/>
+      <c r="A14" s="1">
+        <v>45838</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0.875</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="2"/>
+      <c r="A15" s="1">
+        <v>45838</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="2"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="2"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="2"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="2"/>
+      <c r="A16" s="1">
+        <v>45840</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0.875</v>
+      </c>
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>45840</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>45841</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0.875</v>
+      </c>
+      <c r="C18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>45841</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="C19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
25.06.2025 - maç sonuçları
</commit_message>
<xml_diff>
--- a/data/mac-sonuclari.xlsx
+++ b/data/mac-sonuclari.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yakay\OneDrive\Masaüstü\d-8\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02EE8AAE-DCB6-4591-8867-6582502EE88E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05CF3BDE-4FCE-4EB9-818F-1B0284A7B76C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2370" yWindow="-13620" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Maçlar" sheetId="1" r:id="rId1"/>
@@ -466,8 +466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -702,6 +702,12 @@
       <c r="E10" t="s">
         <v>11</v>
       </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+      <c r="G10">
+        <v>24</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -719,22 +725,28 @@
       <c r="E11" t="s">
         <v>16</v>
       </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>45834</v>
       </c>
       <c r="B12" s="2">
-        <v>0.875</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E12" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -742,16 +754,16 @@
         <v>45834</v>
       </c>
       <c r="B13" s="2">
-        <v>0.91666666666666663</v>
+        <v>0.875</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E13" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
26.06.2025 - maç sonuçları
</commit_message>
<xml_diff>
--- a/data/mac-sonuclari.xlsx
+++ b/data/mac-sonuclari.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yakay\OneDrive\Masaüstü\d-8\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05CF3BDE-4FCE-4EB9-818F-1B0284A7B76C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21927D97-ADE1-4E19-877A-871AEAD3B3F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2370" yWindow="-13620" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -467,7 +467,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -748,6 +748,12 @@
       <c r="E12" t="s">
         <v>20</v>
       </c>
+      <c r="F12">
+        <v>6</v>
+      </c>
+      <c r="G12">
+        <v>7</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -764,6 +770,12 @@
       </c>
       <c r="E13" t="s">
         <v>15</v>
+      </c>
+      <c r="F13">
+        <v>3</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
feat: Oynanmış maçlar için Maçı İzle butonları eklendi
- Excel dosyasında Link sütunu desteği eklendi
- MatchList componentine YouTube video linklerine yönlendiren butonlar eklendi
- process-excel.js scripti Link sütununu okuyacak şekilde güncellendi
- Sadece video linki olan oynanmış maçlarda buton görünür
- Yeni sekmede açılır ve mobil uyumlu tasarım
- create-excel-template.js dosyasına Link sütunu eklendi
</commit_message>
<xml_diff>
--- a/data/mac-sonuclari.xlsx
+++ b/data/mac-sonuclari.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yakay\OneDrive\Masaüstü\d-8\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21927D97-ADE1-4E19-877A-871AEAD3B3F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35057230-6C46-4B38-8812-1DA6A90F918C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2370" yWindow="-13620" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2985" yWindow="-13920" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Maçlar" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="34">
   <si>
     <t>Tarih</t>
   </si>
@@ -31,10 +31,10 @@
     <t>Grup</t>
   </si>
   <si>
-    <t>Takim1</t>
-  </si>
-  <si>
-    <t>Takim2</t>
+    <t>Takım1</t>
+  </si>
+  <si>
+    <t>Takım2</t>
   </si>
   <si>
     <t>Skor1</t>
@@ -43,6 +43,9 @@
     <t>Skor2</t>
   </si>
   <si>
+    <t>Link</t>
+  </si>
+  <si>
     <t>Ahmet Minguzzi Grubu</t>
   </si>
   <si>
@@ -52,6 +55,9 @@
     <t>Ravager</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>Çirihtalar</t>
   </si>
   <si>
@@ -76,6 +82,9 @@
     <t>Narin Güran Grubu</t>
   </si>
   <si>
+    <t>Fortuna United</t>
+  </si>
+  <si>
     <t>Of FK</t>
   </si>
   <si>
@@ -85,7 +94,34 @@
     <t>61.Alay</t>
   </si>
   <si>
-    <t>Fortuna United</t>
+    <t>https://youtu.be/nqf2RPCnLGw</t>
+  </si>
+  <si>
+    <t>https://youtu.be/4udqsX0EYMA</t>
+  </si>
+  <si>
+    <t>https://youtu.be/WNBXhqiaTQQ</t>
+  </si>
+  <si>
+    <t>https://youtu.be/A4Zsh-nURAQ</t>
+  </si>
+  <si>
+    <t>https://youtu.be/Mfes4jxAMQ8</t>
+  </si>
+  <si>
+    <t>https://youtu.be/OUcjYh9v4l0</t>
+  </si>
+  <si>
+    <t>https://youtu.be/0CQJbBd-DCo</t>
+  </si>
+  <si>
+    <t>https://youtu.be/xkq854V1MVs</t>
+  </si>
+  <si>
+    <t>https://youtu.be/HZrAxbLTD4E</t>
+  </si>
+  <si>
+    <t>https://youtu.be/uAyL-1RXy30</t>
   </si>
 </sst>
 </file>
@@ -464,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -477,9 +513,10 @@
     <col min="3" max="3" width="20.875" customWidth="1"/>
     <col min="4" max="5" width="18.875" customWidth="1"/>
     <col min="6" max="7" width="8.875" customWidth="1"/>
+    <col min="8" max="8" width="40.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -501,8 +538,11 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45824</v>
       </c>
@@ -510,13 +550,13 @@
         <v>0.875</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2">
         <v>15</v>
@@ -524,8 +564,11 @@
       <c r="G2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45824</v>
       </c>
@@ -533,13 +576,13 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
         <v>21</v>
-      </c>
-      <c r="E3" t="s">
-        <v>18</v>
       </c>
       <c r="F3">
         <v>4</v>
@@ -547,8 +590,11 @@
       <c r="G3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45826</v>
       </c>
@@ -556,13 +602,13 @@
         <v>0.875</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F4">
         <v>6</v>
@@ -570,8 +616,11 @@
       <c r="G4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45826</v>
       </c>
@@ -579,13 +628,13 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F5">
         <v>2</v>
@@ -593,8 +642,11 @@
       <c r="G5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45827</v>
       </c>
@@ -602,13 +654,13 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F6">
         <v>2</v>
@@ -616,8 +668,11 @@
       <c r="G6">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>45827</v>
       </c>
@@ -625,13 +680,13 @@
         <v>0.875</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F7">
         <v>2</v>
@@ -639,8 +694,11 @@
       <c r="G7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>45831</v>
       </c>
@@ -648,13 +706,13 @@
         <v>0.875</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F8">
         <v>6</v>
@@ -662,8 +720,11 @@
       <c r="G8">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>45831</v>
       </c>
@@ -671,13 +732,13 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -685,8 +746,11 @@
       <c r="G9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>45833</v>
       </c>
@@ -694,13 +758,13 @@
         <v>0.875</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F10">
         <v>3</v>
@@ -708,8 +772,11 @@
       <c r="G10">
         <v>24</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>45833</v>
       </c>
@@ -717,13 +784,13 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E11" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F11">
         <v>1</v>
@@ -731,8 +798,11 @@
       <c r="G11">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>45834</v>
       </c>
@@ -740,13 +810,13 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E12" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F12">
         <v>6</v>
@@ -754,8 +824,11 @@
       <c r="G12">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>45834</v>
       </c>
@@ -763,13 +836,13 @@
         <v>0.875</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E13" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F13">
         <v>3</v>
@@ -777,8 +850,11 @@
       <c r="G13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>45838</v>
       </c>
@@ -786,16 +862,19 @@
         <v>0.875</v>
       </c>
       <c r="C14" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D14" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E14" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>45838</v>
       </c>
@@ -803,16 +882,19 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="C15" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="H15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>45840</v>
       </c>
@@ -820,16 +902,19 @@
         <v>0.875</v>
       </c>
       <c r="C16" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="H16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>45840</v>
       </c>
@@ -837,16 +922,19 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="C17" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D17" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>45841</v>
       </c>
@@ -854,16 +942,19 @@
         <v>0.875</v>
       </c>
       <c r="C18" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D18" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="H18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>45841</v>
       </c>
@@ -871,19 +962,22 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="C19" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D19" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E19" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="H19" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:G1" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:H1 H12:H19" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Of fk vs 61.Alay - Maç linki eklendi
</commit_message>
<xml_diff>
--- a/data/mac-sonuclari.xlsx
+++ b/data/mac-sonuclari.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yakay\OneDrive\Masaüstü\d-8\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35057230-6C46-4B38-8812-1DA6A90F918C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6B66FC3-C32F-48D7-BC0A-9B3F6ABF2F8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2985" yWindow="-13920" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Maçlar" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="35">
   <si>
     <t>Tarih</t>
   </si>
@@ -122,6 +122,9 @@
   </si>
   <si>
     <t>https://youtu.be/uAyL-1RXy30</t>
+  </si>
+  <si>
+    <t>https://youtu.be/j0ONT2EiueM</t>
   </si>
 </sst>
 </file>
@@ -503,7 +506,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -825,7 +828,7 @@
         <v>7</v>
       </c>
       <c r="H12" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -977,7 +980,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:H1 H12:H19" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:H1 H13:H19" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Armedospor vs Of 1461 - Maç linki eklendi. Ajans Of vs Kural Kesiciler maç sonucu eklendi
</commit_message>
<xml_diff>
--- a/data/mac-sonuclari.xlsx
+++ b/data/mac-sonuclari.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yakay\OneDrive\Masaüstü\d-8\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6B66FC3-C32F-48D7-BC0A-9B3F6ABF2F8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{856DAB6E-D0DB-40A9-A074-2FD60D82DDA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28020" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Maçlar" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="36">
   <si>
     <t>Tarih</t>
   </si>
@@ -125,16 +125,27 @@
   </si>
   <si>
     <t>https://youtu.be/j0ONT2EiueM</t>
+  </si>
+  <si>
+    <t>https://youtu.be/r6AEVdp_RAM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -157,15 +168,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Köprü" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -506,7 +520,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -827,7 +841,7 @@
       <c r="G12">
         <v>7</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="3" t="s">
         <v>34</v>
       </c>
     </row>
@@ -854,7 +868,7 @@
         <v>1</v>
       </c>
       <c r="H13" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -873,6 +887,12 @@
       <c r="E14" t="s">
         <v>13</v>
       </c>
+      <c r="F14">
+        <v>3</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
       <c r="H14" t="s">
         <v>11</v>
       </c>
@@ -978,9 +998,12 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H12" r:id="rId1" xr:uid="{07062D61-305A-4ED9-9120-3C848D49B518}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:H1 H13:H19" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:H1 H14:H19" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
30.06.2025 - maç sonuçları
</commit_message>
<xml_diff>
--- a/data/mac-sonuclari.xlsx
+++ b/data/mac-sonuclari.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yakay\OneDrive\Masaüstü\d-8\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{856DAB6E-D0DB-40A9-A074-2FD60D82DDA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F011A95-3692-48D9-A6B1-E62A13275037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28020" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -520,7 +520,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -913,6 +913,12 @@
       <c r="E15" t="s">
         <v>23</v>
       </c>
+      <c r="F15">
+        <v>3</v>
+      </c>
+      <c r="G15">
+        <v>3</v>
+      </c>
       <c r="H15" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
30.06.2025 - maç kayıtları eklendi
</commit_message>
<xml_diff>
--- a/data/mac-sonuclari.xlsx
+++ b/data/mac-sonuclari.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yakay\OneDrive\Masaüstü\d-8\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F011A95-3692-48D9-A6B1-E62A13275037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41F0CA44-9086-478D-9139-2C6D1B67EB78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28020" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="38">
   <si>
     <t>Tarih</t>
   </si>
@@ -128,6 +128,12 @@
   </si>
   <si>
     <t>https://youtu.be/r6AEVdp_RAM</t>
+  </si>
+  <si>
+    <t>https://youtu.be/rbFAYTWC6z4</t>
+  </si>
+  <si>
+    <t>https://youtu.be/mjBKimYNaCk</t>
   </si>
 </sst>
 </file>
@@ -520,7 +526,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -894,7 +900,7 @@
         <v>1</v>
       </c>
       <c r="H14" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -920,7 +926,7 @@
         <v>3</v>
       </c>
       <c r="H15" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1009,7 +1015,7 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:H1 H14:H19" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:H1 H16:H19" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
02.07.2025 - maç sonuçları eklendi
</commit_message>
<xml_diff>
--- a/data/mac-sonuclari.xlsx
+++ b/data/mac-sonuclari.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yakay\OneDrive\Masaüstü\d-8\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41F0CA44-9086-478D-9139-2C6D1B67EB78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93E906C8-EFBD-494B-BF2A-0033D23F891C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28020" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -526,7 +526,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -945,6 +945,12 @@
       <c r="E16" t="s">
         <v>17</v>
       </c>
+      <c r="F16">
+        <v>5</v>
+      </c>
+      <c r="G16">
+        <v>4</v>
+      </c>
       <c r="H16" t="s">
         <v>11</v>
       </c>
@@ -964,6 +970,12 @@
       </c>
       <c r="E17" t="s">
         <v>12</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>3</v>
       </c>
       <c r="H17" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
03.07.2025 - maç sonuçları eklendi
</commit_message>
<xml_diff>
--- a/data/mac-sonuclari.xlsx
+++ b/data/mac-sonuclari.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yakay\OneDrive\Masaüstü\d-8\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93E906C8-EFBD-494B-BF2A-0033D23F891C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB933A0-5969-4EA3-A36F-BCCABDC865B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28020" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5205" yWindow="1890" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Maçlar" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="39">
   <si>
     <t>Tarih</t>
   </si>
@@ -134,6 +134,9 @@
   </si>
   <si>
     <t>https://youtu.be/mjBKimYNaCk</t>
+  </si>
+  <si>
+    <t>https://youtu.be/LJGmM-PJz-g</t>
   </si>
 </sst>
 </file>
@@ -526,7 +529,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -952,7 +955,7 @@
         <v>4</v>
       </c>
       <c r="H16" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -997,6 +1000,12 @@
       <c r="E18" t="s">
         <v>22</v>
       </c>
+      <c r="F18">
+        <v>17</v>
+      </c>
+      <c r="G18">
+        <v>3</v>
+      </c>
       <c r="H18" t="s">
         <v>11</v>
       </c>
@@ -1016,6 +1025,12 @@
       </c>
       <c r="E19" t="s">
         <v>18</v>
+      </c>
+      <c r="F19">
+        <v>3</v>
+      </c>
+      <c r="G19">
+        <v>7</v>
       </c>
       <c r="H19" t="s">
         <v>11</v>
@@ -1027,7 +1042,7 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:H1 H16:H19" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:H1 H17:H19" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
03.07.2025 - Of FK vs Ofside - Maç Görüntüleri eklendi
</commit_message>
<xml_diff>
--- a/data/mac-sonuclari.xlsx
+++ b/data/mac-sonuclari.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yakay\OneDrive\Masaüstü\d-8\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB933A0-5969-4EA3-A36F-BCCABDC865B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6ED11D5-948F-48E6-B318-C985086F9423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5205" yWindow="1890" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5550" yWindow="2235" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Maçlar" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="40">
   <si>
     <t>Tarih</t>
   </si>
@@ -137,6 +137,9 @@
   </si>
   <si>
     <t>https://youtu.be/LJGmM-PJz-g</t>
+  </si>
+  <si>
+    <t>https://youtu.be/jZrjaidowko</t>
   </si>
 </sst>
 </file>
@@ -529,7 +532,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1007,7 +1010,7 @@
         <v>3</v>
       </c>
       <c r="H18" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1042,7 +1045,7 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:H1 H17:H19" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:H1 H17 H19" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Kupa yolu maçları girildi ve Hubuş FK vs Armedospor maçı kaydı eklendi
</commit_message>
<xml_diff>
--- a/data/mac-sonuclari.xlsx
+++ b/data/mac-sonuclari.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yakay\OneDrive\Masaüstü\d-8\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6ED11D5-948F-48E6-B318-C985086F9423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEDF49BB-E8B4-4936-A8F5-007805ECB4A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5550" yWindow="2235" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Maçlar" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="41">
   <si>
     <t>Tarih</t>
   </si>
@@ -140,6 +140,9 @@
   </si>
   <si>
     <t>https://youtu.be/jZrjaidowko</t>
+  </si>
+  <si>
+    <t>https://youtu.be/6QokPQ6a1yA</t>
   </si>
 </sst>
 </file>
@@ -532,7 +535,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1036,7 +1039,7 @@
         <v>7</v>
       </c>
       <c r="H19" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1045,7 +1048,7 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:H1 H17 H19" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:H1 H17" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>